<commit_message>
hoàn thành file checklist
</commit_message>
<xml_diff>
--- a/Testing/checklist.xlsx
+++ b/Testing/checklist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>Danh sách các Testcase</t>
   </si>
@@ -125,6 +125,60 @@
   </si>
   <si>
     <t>Nhập địa chỉ trang tạo công việc (sau khi đăng nhập)</t>
+  </si>
+  <si>
+    <t>Nhập đúng và đầy đủ thông tin công việc</t>
+  </si>
+  <si>
+    <t>Nhập đầy đủ thông tin nhưng vi phạm qui định các trường</t>
+  </si>
+  <si>
+    <t>Trang danh sách công việc</t>
+  </si>
+  <si>
+    <t>Nhập địa chỉ trang danh sách công việc (trước khi đăng nhập)</t>
+  </si>
+  <si>
+    <t>Nhập địa chỉ trang danh sách công việc (sau khi đăng nhập)</t>
+  </si>
+  <si>
+    <t>Chức năng Deactive</t>
+  </si>
+  <si>
+    <t>Trang admin</t>
+  </si>
+  <si>
+    <t>Nhập địa chỉ trang admin (trước khi đăng nhập tài khoản admin)</t>
+  </si>
+  <si>
+    <t>Nhập địa chỉ trang admin (sau khi đăng nhập tài khoản admin)</t>
+  </si>
+  <si>
+    <t>Nhập địa chỉ trang admin (sau khi đăng nhập tài khoản thường)</t>
+  </si>
+  <si>
+    <t>Chọn "User"</t>
+  </si>
+  <si>
+    <t>Chọn người dùng</t>
+  </si>
+  <si>
+    <t>Chọn "Company"</t>
+  </si>
+  <si>
+    <t>Chức năng Xóa</t>
+  </si>
+  <si>
+    <t>Chọn "Skill"</t>
+  </si>
+  <si>
+    <t>Chọn "Degree"</t>
+  </si>
+  <si>
+    <t>Chọn "Admin"</t>
+  </si>
+  <si>
+    <t>Chức năng Download file log</t>
   </si>
 </sst>
 </file>
@@ -140,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,15 +226,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,26 +540,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -512,12 +573,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -552,11 +613,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -599,11 +660,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -670,11 +731,11 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -749,11 +810,11 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -820,11 +881,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -899,24 +960,379 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>44</v>
+      </c>
       <c r="B53" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>45</v>
+      </c>
       <c r="B54" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>47</v>
+      </c>
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>50</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>51</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>54</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>55</v>
+      </c>
+      <c r="B65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>56</v>
+      </c>
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>57</v>
+      </c>
+      <c r="B67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>58</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>59</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>62</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>63</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>64</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>65</v>
+      </c>
+      <c r="B76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>66</v>
+      </c>
+      <c r="B77" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>67</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="4"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>68</v>
+      </c>
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>69</v>
+      </c>
+      <c r="B80" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>70</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>71</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="4"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>72</v>
+      </c>
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>73</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>74</v>
+      </c>
+      <c r="B85" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>75</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" s="4"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>76</v>
+      </c>
+      <c r="B87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>77</v>
+      </c>
+      <c r="B88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>78</v>
+      </c>
+      <c r="B89" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>79</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>80</v>
+      </c>
+      <c r="B91" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>81</v>
+      </c>
+      <c r="B92" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>82</v>
+      </c>
+      <c r="B93" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>83</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>84</v>
+      </c>
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>85</v>
+      </c>
+      <c r="B96" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>86</v>
+      </c>
+      <c r="B97" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A74:C74"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A42:C42"/>

</xml_diff>